<commit_message>
Updated test cases and defect report
</commit_message>
<xml_diff>
--- a/Reports/Defect Report On OpenCart Ecommerce Website.xlsx
+++ b/Reports/Defect Report On OpenCart Ecommerce Website.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f8df42fb1d994e7/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{C7F0AA17-30ED-4AB0-9FC0-471A05343913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC1C6544-9768-4F89-8F46-1FA44CC06DFF}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{C7F0AA17-30ED-4AB0-9FC0-471A05343913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13607E03-6A25-4833-B982-5E1F283F41A3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{6703EAF1-097C-4C7D-AD54-2FB592AB9A71}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <r>
       <t>Ø</t>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>TC_006</t>
-  </si>
-  <si>
-    <t>TC_Cart_006</t>
   </si>
   <si>
     <t>Vaishali Mam(Manager name)</t>
@@ -308,6 +305,9 @@
     <t>Def_opencart_003</t>
   </si>
   <si>
+    <t>TC_011</t>
+  </si>
+  <si>
     <t>Login Module</t>
   </si>
   <si>
@@ -353,6 +353,9 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>TC_Cart_011</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -772,10 +775,10 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="94">
@@ -786,7 +789,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>34</v>
@@ -797,10 +800,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>21</v>
@@ -811,10 +814,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>36</v>
@@ -825,10 +828,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -842,7 +845,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>37</v>
@@ -942,13 +945,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="22.5">
@@ -961,13 +964,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>